<commit_message>
Hyper tension file changes added -pavithra
</commit_message>
<xml_diff>
--- a/target/test-classes/TestData/8WebScrappershypothyroiddata.xlsx
+++ b/target/test-classes/TestData/8WebScrappershypothyroiddata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavit\eclipse-jobpracticespace\8WebScrappers\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727B1E19-A237-41AD-9546-227F8B0667CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DB8C1A-D938-4A85-8062-1236E4586339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5DBEED5C-9134-49E0-A613-04568B1A6B57}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="286">
   <si>
     <t>RecipeId</t>
   </si>
@@ -102,39 +102,6 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/recipes-for-hypothyroidism-veg-diet-indian-recipes-849</t>
-  </si>
-  <si>
-    <t>40603</t>
-  </si>
-  <si>
-    <t>Baingan Bhaja, Bengali Begun Bhaja</t>
-  </si>
-  <si>
-    <t>For Baingan Bhaja
-18 big brinjal (baingan / eggplant) slices
-2 tsp chilli powder
-1/2 tsp turmeric powder (haldi)
-1 tbsp lemon juice
-1/4 cup besan (bengal gram flour)
-salt to taste
-2 tsp oil for greasing and cooking</t>
-  </si>
-  <si>
-    <t>10 mins</t>
-  </si>
-  <si>
-    <t>20 mins</t>
-  </si>
-  <si>
-    <t>For baingan bhaja
-To make baingan bhaja, combine the chilli powder, turmeric powder, lemon juice, besan, salt and 2 tbsp of water in a deep bowl and mix well.
-Add the baingan slices and mix well. Keep aside.
-Heat a non-stick tava (griddle), grease it with ½ tsp of oil, arrange half the baingan slices and cook using ½ tsp of oil on both the sides till golden brown in colour.
-Repeat step 3 to make 1 more batch.
-Serve the baingan bhaja immediately.</t>
-  </si>
-  <si>
-    <t>Protein 5.5 g</t>
   </si>
   <si>
     <t>5292</t>
@@ -158,6 +125,9 @@
 salt to taste
 For The Garnish
 2 tbsp chopped coriander (dhania)</t>
+  </si>
+  <si>
+    <t>10 mins</t>
   </si>
   <si>
     <t>25 mins</t>
@@ -262,6 +232,9 @@
     <t>5 mins</t>
   </si>
   <si>
+    <t>20 mins</t>
+  </si>
+  <si>
     <t>For buckwheat dosas
 To make buckwheat dosas, combine the buckwheat and urad dal in a mixer and blend to a fine powder.
 Transfer the powder in a deep bowl and keep aside.
@@ -396,85 +369,6 @@
   </si>
   <si>
     <t>Fiber 3 g</t>
-  </si>
-  <si>
-    <t>42333</t>
-  </si>
-  <si>
-    <t>Egg Paratha</t>
-  </si>
-  <si>
-    <t>For The Parathas
-3/4 cup whole wheat flour (gehun ka atta)
-1/2 tsp carom seeds (ajwain)
-salt to taste
-whole wheat flour (gehun ka atta) for rolling
-1/2 tsp ghee for spreading
-1 tsp oil for cooking
-For The Egg Mixture
-3 eggs
-1/4 cup finely chopped onions
-1/4 cup finely chopped tomatoes
-2 tbsp finely chopped coriander (dhania)
-1 tsp finely chopped green chillies
-salt to taste
-Other Ingredients For Egg Paratha
-2 tsp oil for greasing
-2 tsp oil for cooking</t>
-  </si>
-  <si>
-    <t>For the parathas
-Combine all the ingredients in a deep bowl and knead into a soft dough using enough water.
-Divide the dough into 2 equal portions.
-Roll a portion of the dough into 150 mm. (6”) diameter circle using a little whole wheat flour for rolling. Spread ¼ tsp of ghee evenly over it.
-Fold over from one end to another end slightly overlapping each other.
-Then fold again from one end to another end overlapping each other.
-Roll again into a 175 mm. (7”) diameter circle using a little whole wheat flour for rolling.
-Heat a non-stick tava (griddle) and cook the paratha using ½ tsp of oil till it turns golden brown in colour from both the sides
-Repeat steps 3 to 7 to make 1 more paratha. Keep aside.
-For the egg mixture
-Break the eggs in a deep bowl and beat well using a fork.
-Add all the other ingredients and beat well. Keep aside.
-How to proceed
-To make egg paratha, heat a non-stick tava (griddle) and grease it using 1 tsp of oil. Pour half the egg mixture on it.
-Place a prepared paratha on it and press it lightly. Cook using 1 tsp of oil.
-Turnover and cook again till it is cooked.
-Cut into 4 equal portions using a cutter or a sharp knife.
-Repeat steps 1 to 4 to make 1 more egg paratha.
-Serve egg paratha immediately.</t>
-  </si>
-  <si>
-    <t>Fat 2.1 g</t>
-  </si>
-  <si>
-    <t>7468</t>
-  </si>
-  <si>
-    <t>Fenugreek and Mushroom Brown Rice</t>
-  </si>
-  <si>
-    <t>2 cups finely chopped fenugreek (methi) leaves
-1 cup sliced mushrooms (khumbh)
-1 cup brown rice
-2 tsp oil
-2 tsp finely chopped green chillies
-1 tsp finely chopped ginger (adrak)
-1 tbsp finely chopped garlic (lehsun)
-1 cup finely chopped onions
-1/2 cup finely chopped tomatoes
-1/2 cup brinjal (baingan / eggplant) cubes
-1/2 cup surti papdi seeds (fresh vaal seeds)
-1/2 tsp chilli powder
-salt to taste
-For The Garnish
-2 tbsp finely chopped coriander (dhania)</t>
-  </si>
-  <si>
-    <t>Heat the oil in a pressure cooker, add the green chillies, ginger, garlic, and onions and sauté on a medium flame for 2 minutes.
-Add the fenugreek leaves, mushrooms, tomatoes, brinjals, surti papadi seeds,and chilli powder, mix well and cook on a medium flame for 1 to 2 minutes, while stirring occasionally.
-Add the brown rice, 2¼ cups of hot water and salt, mix well and pressure cook for 4 whistles.
-Allow the steam to escape before opening the lid.
-Serve hot garnished with coriander.</t>
   </si>
   <si>
     <t>22378</t>
@@ -1389,45 +1283,6 @@
   </si>
   <si>
     <t>Protein 4.4 g</t>
-  </si>
-  <si>
-    <t>6213</t>
-  </si>
-  <si>
-    <t>Apple Magic, Lemony Apple Juice</t>
-  </si>
-  <si>
-    <t>For Bhindi Masala
-20 tender ladies finger (bhindi)
-2 tbsp besan (bengal gram flour)
-2 tsp oil
-For The Bhindi Masala Paste
-1/2 cup roughly chopped onions
-1 cup chopped coriander (dhania)
-2 tsp ginger-green chilli paste
-1/2 tsp turmeric powder (haldi)
-1 tbsp coriander-cumin seeds (dhania-jeera) powder
-1 tsp garam masala
-2 tsp roasted sesame seeds (til)
-1 tbsp lemon juice
-salt to taste
-For Serving With Bhindi Masala
-rotis/parathas</t>
-  </si>
-  <si>
-    <t>For the bhindi masala paste
-Combine all the ingredients and 2 tbsp of water in a mixer and blend till smooth.
-Transfer the mixture into a deep bowl, add the besan and mix well. Keep aside.
-How to proceed to make bhindi masala
-To make bhindi masala, wash, dry and slit the bhindi lengthwise.
-Stuff each bhindi with a little prepared paste. Keep the remaining paste aside.
-Heat a non-stick tava (griddle), put the remaining paste and 2 tbsp of water and sauté on a medium flame for 2 minutes.
-Add the stuffed bhindis and sauté on a medium flame for 4 minutes.
-Cover with a lid and cook on a medium flame for 6 to 8 minutes, while stirring occasionally.
-Serve the bhindi masala hot with rotis or parathas.</t>
-  </si>
-  <si>
-    <t>Carbohydrates 44.4 g</t>
   </si>
   <si>
     <t>22206</t>
@@ -2123,7 +1978,7 @@
   <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AY51"/>
+      <selection activeCell="A2" sqref="A2:AY64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2193,53 +2048,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s" s="0">
         <v>17</v>
@@ -2247,25 +2076,25 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s" s="0">
         <v>17</v>
@@ -2273,25 +2102,25 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J6" t="s" s="0">
         <v>17</v>
@@ -2299,25 +2128,25 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="I7" t="s" s="0">
         <v>42</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>47</v>
       </c>
       <c r="J7" t="s" s="0">
         <v>17</v>
@@ -2325,25 +2154,25 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J8" t="s" s="0">
         <v>17</v>
@@ -2351,25 +2180,25 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J9" t="s" s="0">
         <v>17</v>
@@ -2377,25 +2206,25 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J10" t="s" s="0">
         <v>17</v>
@@ -2403,91 +2232,39 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J11" t="s" s="0">
         <v>17</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="F12" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H12" t="s" s="0">
-        <v>73</v>
-      </c>
-      <c r="I12" t="s" s="0">
-        <v>74</v>
-      </c>
-      <c r="J12" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>77</v>
-      </c>
-      <c r="F13" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H13" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="I13" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="J13" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="F14" t="s" s="0">
         <v>13</v>
@@ -2496,10 +2273,10 @@
         <v>13</v>
       </c>
       <c r="H14" t="s" s="0">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="I14" t="s" s="0">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="J14" t="s" s="0">
         <v>17</v>
@@ -2507,25 +2284,25 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F15" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="H15" t="s" s="0">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="I15" t="s" s="0">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="J15" t="s" s="0">
         <v>17</v>
@@ -2533,25 +2310,25 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="J16" t="s" s="0">
         <v>17</v>
@@ -2559,25 +2336,25 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H17" t="s" s="0">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="I17" t="s" s="0">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="J17" t="s" s="0">
         <v>17</v>
@@ -2585,25 +2362,25 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F18" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G18" t="s" s="0">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H18" t="s" s="0">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="I18" t="s" s="0">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J18" t="s" s="0">
         <v>17</v>
@@ -2611,25 +2388,25 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="F19" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J19" t="s" s="0">
         <v>17</v>
@@ -2637,25 +2414,25 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="G20" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H20" t="s" s="0">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="I20" t="s" s="0">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="J20" t="s" s="0">
         <v>17</v>
@@ -2663,25 +2440,25 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="E21" t="s" s="0">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="F21" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G21" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H21" t="s" s="0">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="I21" t="s" s="0">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="J21" t="s" s="0">
         <v>17</v>
@@ -2689,25 +2466,25 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G22" t="s" s="0">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="H22" t="s" s="0">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="I22" t="s" s="0">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="J22" t="s" s="0">
         <v>17</v>
@@ -2715,25 +2492,25 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="F23" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H23" t="s" s="0">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="I23" t="s" s="0">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="J23" t="s" s="0">
         <v>17</v>
@@ -2741,25 +2518,25 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="F24" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G24" t="s" s="0">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H24" t="s" s="0">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="I24" t="s" s="0">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="J24" t="s" s="0">
         <v>17</v>
@@ -2767,195 +2544,195 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="F25" t="s" s="0">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G25" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H25" t="s" s="0">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="I25" t="s" s="0">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J25" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F26" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G26" t="s" s="0">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="H26" t="s" s="0">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="I26" t="s" s="0">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="J26" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="F27" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G27" t="s" s="0">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="H27" t="s" s="0">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="I27" t="s" s="0">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="J27" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F28" t="s" s="0">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G28" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H28" t="s" s="0">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="I28" t="s" s="0">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="J28" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E30" t="s" s="0">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="F30" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G30" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H30" t="s" s="0">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="I30" t="s" s="0">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="J30" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="F31" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G31" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H31" t="s" s="0">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="I31" t="s" s="0">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="J31" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="F32" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G32" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="E33" t="s" s="0">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="F33" t="s" s="0">
         <v>21</v>
@@ -2964,24 +2741,24 @@
         <v>21</v>
       </c>
       <c r="H33" t="s" s="0">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="I33" t="s" s="0">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="J33" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="E34" t="s" s="0">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="F34" t="s" s="0">
         <v>13</v>
@@ -2990,24 +2767,24 @@
         <v>13</v>
       </c>
       <c r="H34" t="s" s="0">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="I34" t="s" s="0">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="J34" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="E35" t="s" s="0">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F35" t="s" s="0">
         <v>21</v>
@@ -3016,24 +2793,24 @@
         <v>13</v>
       </c>
       <c r="H35" t="s" s="0">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="I35" t="s" s="0">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="J35" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="F36" t="s" s="0">
         <v>21</v>
@@ -3042,310 +2819,284 @@
         <v>13</v>
       </c>
       <c r="H36" t="s" s="0">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="I36" t="s" s="0">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="J36" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="E37" t="s" s="0">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="F37" t="s" s="0">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G37" t="s" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H37" t="s" s="0">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="I37" t="s" s="0">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J37" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="E38" t="s" s="0">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="F38" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G38" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H38" t="s" s="0">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="I38" t="s" s="0">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="J38" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="E39" t="s" s="0">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="F39" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G39" t="s" s="0">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="H39" t="s" s="0">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="I39" t="s" s="0">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="J39" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="E40" t="s" s="0">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="F40" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="G40" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="G40" t="s" s="0">
-        <v>28</v>
-      </c>
       <c r="H40" t="s" s="0">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="I40" t="s" s="0">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="J40" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="E41" t="s" s="0">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="F41" t="s" s="0">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G41" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H41" t="s" s="0">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I41" t="s" s="0">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="J41" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="E42" t="s" s="0">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="F42" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G42" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H42" t="s" s="0">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="I42" t="s" s="0">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="J42" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="E43" t="s" s="0">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F43" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G43" t="s" s="0">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="H43" t="s" s="0">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="I43" t="s" s="0">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J43" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="F44" t="s" s="0">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G44" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H44" t="s" s="0">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="I44" t="s" s="0">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="J44" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="E45" t="s" s="0">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="F45" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G45" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H45" t="s" s="0">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="I45" t="s" s="0">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="J45" t="s" s="0">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="0">
-        <v>239</v>
-      </c>
-      <c r="B46" t="s" s="0">
-        <v>240</v>
-      </c>
-      <c r="E46" t="s" s="0">
-        <v>241</v>
-      </c>
-      <c r="F46" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G46" t="s" s="0">
-        <v>124</v>
-      </c>
-      <c r="H46" t="s" s="0">
-        <v>242</v>
-      </c>
-      <c r="I46" t="s" s="0">
-        <v>243</v>
-      </c>
-      <c r="J46" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="E47" t="s" s="0">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="F47" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G47" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H47" t="s" s="0">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="I47" t="s" s="0">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="J47" t="s" s="0">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="E48" t="s" s="0">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="F48" t="s" s="0">
         <v>13</v>
@@ -3354,102 +3105,102 @@
         <v>21</v>
       </c>
       <c r="H48" t="s" s="0">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="I48" t="s" s="0">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="J48" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="E49" t="s" s="0">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="F49" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G49" t="s" s="0">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="H49" t="s" s="0">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="I49" t="s" s="0">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J49" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="E50" t="s" s="0">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="F50" t="s" s="0">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="G50" t="s" s="0">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="H50" t="s" s="0">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="I50" t="s" s="0">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="J50" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="E51" t="s" s="0">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="F51" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G51" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H51" t="s" s="0">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="I51" t="s" s="0">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="J51" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="E53" t="s" s="0">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="F53" t="s" s="0">
         <v>13</v>
@@ -3458,169 +3209,169 @@
         <v>21</v>
       </c>
       <c r="H53" t="s" s="0">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="I53" t="s" s="0">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="J53" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="E54" t="s" s="0">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="F54" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G54" t="s" s="0">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="H54" t="s" s="0">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="I54" t="s" s="0">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J54" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="E55" t="s" s="0">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="F55" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G55" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H55" t="s" s="0">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="I55" t="s" s="0">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J55" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="E56" t="s" s="0">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G56" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H56" t="s" s="0">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="I56" t="s" s="0">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="J56" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="E57" t="s" s="0">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="F57" t="s" s="0">
         <v>21</v>
       </c>
       <c r="G57" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H57" t="s" s="0">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="I57" t="s" s="0">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="J57" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="E58" t="s" s="0">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="F58" t="s" s="0">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G58" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H58" t="s" s="0">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="I58" t="s" s="0">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="J58" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="E59" t="s" s="0">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="F59" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G59" t="s" s="0">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H59" t="s" s="0">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="I59" t="s" s="0">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="J59" t="s" s="0">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>